<commit_message>
run 1 - unsuccessful
</commit_message>
<xml_diff>
--- a/companies.xlsx
+++ b/companies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavlalam/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavlalam/Library/CloudStorage/GoogleDrive-abhinavlalam@gmail.com/My Drive/[06] Projects/Github/download-logos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36CD3615-4835-4E4C-A689-1C2F802C6129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8C1DBA-C036-2A48-924D-EFFBEBEBA3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2620" windowWidth="27640" windowHeight="16940" xr2:uid="{EBBD451B-AFCE-A447-BA71-731753E57721}"/>
   </bookViews>
@@ -1186,7 +1186,7 @@
   <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>